<commit_message>
added a working code
</commit_message>
<xml_diff>
--- a/My_IPC.xlsx
+++ b/My_IPC.xlsx
@@ -21,9 +21,6 @@
     <t>P/N</t>
   </si>
   <si>
-    <t>АТА&amp;Pos</t>
-  </si>
-  <si>
     <t>A508-28</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>33-40-03-1_Pos.100</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -541,71 +541,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1">
       <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the bot's response when entering the wrong P/N.
</commit_message>
<xml_diff>
--- a/My_IPC.xlsx
+++ b/My_IPC.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>P/N</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>27-50-03-1_Pos.130</t>
+  </si>
+  <si>
+    <t>MB2061SS4W01-CC</t>
+  </si>
+  <si>
+    <t>27-10-01-1_Pos.270</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -644,6 +650,14 @@
       </c>
       <c r="B10" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>